<commit_message>
Add hour weights and discount capital costs I added hour weights to the model to properly weight variable costs and transportation costs. I also added a discount factor to capital costs.
</commit_message>
<xml_diff>
--- a/H2CS2/outputs/output_2region_short.xlsx
+++ b/H2CS2/outputs/output_2region_short.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22a94a39b5425449/Documents/02_School/04_ETH/02_Spring_2023_Semester/06_Case_Study/02_Model/Case-Study-ETH/H2CS2/outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="115_{9D0F99C9-3BAA-40D8-A958-E05AF8775447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17400" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="objective" sheetId="1" r:id="rId1"/>
-    <sheet name="quantity" sheetId="2" r:id="rId2"/>
-    <sheet name="capacity" sheetId="3" r:id="rId3"/>
-    <sheet name="flow" sheetId="4" r:id="rId4"/>
-    <sheet name="mass_balance" sheetId="5" r:id="rId5"/>
+    <sheet name="quantity" r:id="rId5" sheetId="2"/>
+    <sheet name="capacity" r:id="rId6" sheetId="3"/>
+    <sheet name="flow" r:id="rId7" sheetId="4"/>
+    <sheet name="mass_balance" r:id="rId8" sheetId="5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Objective</t>
   </si>
@@ -445,21 +445,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C5D72E-5BC3-4A36-A56D-A46CAC826DBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:1">
       <c r="A2">
-        <v>51.306040683557072</v>
+        <v>14703.746712167798</v>
       </c>
     </row>
   </sheetData>
@@ -468,14 +468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFAA124-D30B-4484-8C00-95D3F216D5D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -489,7 +489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -500,10 +500,10 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -514,10 +514,10 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -528,10 +528,10 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -542,10 +542,10 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -556,10 +556,10 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -570,10 +570,10 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -584,10 +584,10 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -598,10 +598,10 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -612,10 +612,10 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -626,10 +626,10 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -640,10 +640,10 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -654,10 +654,10 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -668,10 +668,10 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.6">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -682,10 +682,10 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -696,10 +696,10 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -710,10 +710,10 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -727,7 +727,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -741,7 +741,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -752,10 +752,10 @@
         <v>11</v>
       </c>
       <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -766,10 +766,10 @@
         <v>11</v>
       </c>
       <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -783,7 +783,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -797,7 +797,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -808,10 +808,10 @@
         <v>11</v>
       </c>
       <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -822,7 +822,7 @@
         <v>11</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -831,14 +831,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B0E38B-0252-48A7-8D57-8E89D0ED1CF8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -863,16 +863,16 @@
         <v>2030</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -880,16 +880,16 @@
         <v>2030</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2.0</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -897,16 +897,16 @@
         <v>2030</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -914,16 +914,16 @@
         <v>2030</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -931,16 +931,16 @@
         <v>2040</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -948,16 +948,16 @@
         <v>2040</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2.0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -965,16 +965,16 @@
         <v>2040</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -982,13 +982,13 @@
         <v>2040</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -997,14 +997,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5DB256-671A-4CA8-8338-8E7B48905995}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1023,10 +1023,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1034,10 +1034,10 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1045,10 +1045,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1056,10 +1056,10 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1067,10 +1067,10 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1078,10 +1078,10 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1089,10 +1089,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1100,10 +1100,10 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1111,10 +1111,10 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1122,10 +1122,10 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1133,10 +1133,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -1153,14 +1153,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB2FBA9-347D-40CE-B2D1-27E6B391076D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1185,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-1000.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1199,10 +1199,10 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>-16.58433701317114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-2021.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1213,10 +1213,10 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>-0.19277164471476571</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-192.7716447147657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1227,10 +1227,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>-1.3494015130033601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-848.5807800343987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1241,10 +1241,10 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>-11.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-511.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1255,10 +1255,10 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>-8.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-2200.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1269,10 +1269,10 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>-0.57831493414429713</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-193.15718800419523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1283,10 +1283,10 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>-0.84819523674496922</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-848.1952367449692</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1297,10 +1297,10 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-500.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1311,10 +1311,10 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>-2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-2200.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1325,10 +1325,10 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>-0.19277164471476571</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.6">
+        <v>-192.7716447147657</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>-0.84819523674496922</v>
+        <v>-848.1952367449692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>